<commit_message>
Acomodar y limpiar basura del gitignore
</commit_message>
<xml_diff>
--- a/migracionWordPressPrestashop/Combos competidores Rerda.xlsx
+++ b/migracionWordPressPrestashop/Combos competidores Rerda.xlsx
@@ -1077,6 +1077,21 @@
             <v>Crear</v>
           </cell>
         </row>
+        <row r="4">
+          <cell r="B4"/>
+          <cell r="C4"/>
+          <cell r="D4"/>
+        </row>
+        <row r="5">
+          <cell r="B5"/>
+          <cell r="C5"/>
+          <cell r="D5"/>
+        </row>
+        <row r="6">
+          <cell r="B6"/>
+          <cell r="C6"/>
+          <cell r="D6"/>
+        </row>
         <row r="7">
           <cell r="A7" t="str">
             <v>MLA836197786</v>
@@ -1511,6 +1526,33 @@
             <v>Crear</v>
           </cell>
         </row>
+        <row r="14">
+          <cell r="B14"/>
+          <cell r="C14"/>
+          <cell r="D14"/>
+        </row>
+        <row r="15">
+          <cell r="A15"/>
+          <cell r="B15"/>
+          <cell r="C15"/>
+          <cell r="D15"/>
+          <cell r="E15"/>
+          <cell r="F15"/>
+          <cell r="G15"/>
+          <cell r="H15"/>
+          <cell r="I15"/>
+          <cell r="J15"/>
+          <cell r="K15"/>
+          <cell r="L15"/>
+          <cell r="M15"/>
+          <cell r="N15"/>
+          <cell r="O15"/>
+          <cell r="P15"/>
+          <cell r="Q15"/>
+          <cell r="R15"/>
+          <cell r="S15"/>
+          <cell r="T15"/>
+        </row>
         <row r="16">
           <cell r="A16" t="str">
             <v>MLA865416644</v>
@@ -1572,6 +1614,28 @@
           <cell r="T16" t="str">
             <v>Crear</v>
           </cell>
+        </row>
+        <row r="17">
+          <cell r="A17"/>
+          <cell r="B17"/>
+          <cell r="C17"/>
+          <cell r="D17"/>
+          <cell r="E17"/>
+          <cell r="F17"/>
+          <cell r="G17"/>
+          <cell r="H17"/>
+          <cell r="I17"/>
+          <cell r="J17"/>
+          <cell r="K17"/>
+          <cell r="L17"/>
+          <cell r="M17"/>
+          <cell r="N17"/>
+          <cell r="O17"/>
+          <cell r="P17"/>
+          <cell r="Q17"/>
+          <cell r="R17"/>
+          <cell r="S17"/>
+          <cell r="T17"/>
         </row>
         <row r="18">
           <cell r="A18" t="str">
@@ -1636,9 +1700,94 @@
           </cell>
         </row>
         <row r="19">
+          <cell r="A19"/>
+          <cell r="B19"/>
+          <cell r="C19"/>
+          <cell r="D19"/>
+          <cell r="E19"/>
+          <cell r="F19"/>
+          <cell r="G19"/>
+          <cell r="H19"/>
+          <cell r="I19"/>
+          <cell r="J19"/>
+          <cell r="K19"/>
+          <cell r="L19"/>
+          <cell r="M19"/>
+          <cell r="N19"/>
+          <cell r="O19"/>
+          <cell r="P19"/>
+          <cell r="Q19"/>
+          <cell r="R19"/>
+          <cell r="S19"/>
           <cell r="T19">
             <v>6000007</v>
           </cell>
+        </row>
+        <row r="20">
+          <cell r="A20"/>
+          <cell r="B20"/>
+          <cell r="C20"/>
+          <cell r="D20"/>
+          <cell r="E20"/>
+          <cell r="F20"/>
+          <cell r="G20"/>
+          <cell r="H20"/>
+          <cell r="I20"/>
+          <cell r="J20"/>
+          <cell r="K20"/>
+          <cell r="L20"/>
+          <cell r="M20"/>
+          <cell r="N20"/>
+          <cell r="O20"/>
+          <cell r="P20"/>
+          <cell r="Q20"/>
+          <cell r="R20"/>
+          <cell r="S20"/>
+          <cell r="T20"/>
+        </row>
+        <row r="21">
+          <cell r="A21"/>
+          <cell r="B21"/>
+          <cell r="C21"/>
+          <cell r="D21"/>
+          <cell r="E21"/>
+          <cell r="F21"/>
+          <cell r="G21"/>
+          <cell r="H21"/>
+          <cell r="I21"/>
+          <cell r="J21"/>
+          <cell r="K21"/>
+          <cell r="L21"/>
+          <cell r="M21"/>
+          <cell r="N21"/>
+          <cell r="O21"/>
+          <cell r="P21"/>
+          <cell r="Q21"/>
+          <cell r="R21"/>
+          <cell r="S21"/>
+          <cell r="T21"/>
+        </row>
+        <row r="22">
+          <cell r="A22"/>
+          <cell r="B22"/>
+          <cell r="C22"/>
+          <cell r="D22"/>
+          <cell r="E22"/>
+          <cell r="F22"/>
+          <cell r="G22"/>
+          <cell r="H22"/>
+          <cell r="I22"/>
+          <cell r="J22"/>
+          <cell r="K22"/>
+          <cell r="L22"/>
+          <cell r="M22"/>
+          <cell r="N22"/>
+          <cell r="O22"/>
+          <cell r="P22"/>
+          <cell r="Q22"/>
+          <cell r="R22"/>
+          <cell r="S22"/>
+          <cell r="T22"/>
         </row>
         <row r="23">
           <cell r="A23" t="str">
@@ -1760,6 +1909,29 @@
           <cell r="S24">
             <v>19</v>
           </cell>
+          <cell r="T24"/>
+        </row>
+        <row r="25">
+          <cell r="A25"/>
+          <cell r="B25"/>
+          <cell r="C25"/>
+          <cell r="D25"/>
+          <cell r="E25"/>
+          <cell r="F25"/>
+          <cell r="G25"/>
+          <cell r="H25"/>
+          <cell r="I25"/>
+          <cell r="J25"/>
+          <cell r="K25"/>
+          <cell r="L25"/>
+          <cell r="M25"/>
+          <cell r="N25"/>
+          <cell r="O25"/>
+          <cell r="P25"/>
+          <cell r="Q25"/>
+          <cell r="R25"/>
+          <cell r="S25"/>
+          <cell r="T25"/>
         </row>
         <row r="26">
           <cell r="A26" t="str">
@@ -1823,6 +1995,28 @@
             <v>Crear</v>
           </cell>
         </row>
+        <row r="27">
+          <cell r="A27"/>
+          <cell r="B27"/>
+          <cell r="C27"/>
+          <cell r="D27"/>
+          <cell r="E27"/>
+          <cell r="F27"/>
+          <cell r="G27"/>
+          <cell r="H27"/>
+          <cell r="I27"/>
+          <cell r="J27"/>
+          <cell r="K27"/>
+          <cell r="L27"/>
+          <cell r="M27"/>
+          <cell r="N27"/>
+          <cell r="O27"/>
+          <cell r="P27"/>
+          <cell r="Q27"/>
+          <cell r="R27"/>
+          <cell r="S27"/>
+          <cell r="T27"/>
+        </row>
         <row r="28">
           <cell r="A28" t="str">
             <v>MLA830416153</v>
@@ -1884,6 +2078,28 @@
           <cell r="T28" t="str">
             <v>Crear</v>
           </cell>
+        </row>
+        <row r="29">
+          <cell r="A29"/>
+          <cell r="B29"/>
+          <cell r="C29"/>
+          <cell r="D29"/>
+          <cell r="E29"/>
+          <cell r="F29"/>
+          <cell r="G29"/>
+          <cell r="H29"/>
+          <cell r="I29"/>
+          <cell r="J29"/>
+          <cell r="K29"/>
+          <cell r="L29"/>
+          <cell r="M29"/>
+          <cell r="N29"/>
+          <cell r="O29"/>
+          <cell r="P29"/>
+          <cell r="Q29"/>
+          <cell r="R29"/>
+          <cell r="S29"/>
+          <cell r="T29"/>
         </row>
         <row r="30">
           <cell r="A30" t="str">
@@ -1947,6 +2163,33 @@
             <v>Crear</v>
           </cell>
         </row>
+        <row r="31">
+          <cell r="B31"/>
+          <cell r="C31"/>
+          <cell r="D31"/>
+        </row>
+        <row r="32">
+          <cell r="A32"/>
+          <cell r="B32"/>
+          <cell r="C32"/>
+          <cell r="D32"/>
+          <cell r="E32"/>
+          <cell r="F32"/>
+          <cell r="G32"/>
+          <cell r="H32"/>
+          <cell r="I32"/>
+          <cell r="J32"/>
+          <cell r="K32"/>
+          <cell r="L32"/>
+          <cell r="M32"/>
+          <cell r="N32"/>
+          <cell r="O32"/>
+          <cell r="P32"/>
+          <cell r="Q32"/>
+          <cell r="R32"/>
+          <cell r="S32"/>
+          <cell r="T32"/>
+        </row>
         <row r="33">
           <cell r="A33" t="str">
             <v>MLA874830388</v>
@@ -2133,6 +2376,28 @@
             <v>Crear</v>
           </cell>
         </row>
+        <row r="36">
+          <cell r="A36"/>
+          <cell r="B36"/>
+          <cell r="C36"/>
+          <cell r="D36"/>
+          <cell r="E36"/>
+          <cell r="F36"/>
+          <cell r="G36"/>
+          <cell r="H36"/>
+          <cell r="I36"/>
+          <cell r="J36"/>
+          <cell r="K36"/>
+          <cell r="L36"/>
+          <cell r="M36"/>
+          <cell r="N36"/>
+          <cell r="O36"/>
+          <cell r="P36"/>
+          <cell r="Q36"/>
+          <cell r="R36"/>
+          <cell r="S36"/>
+          <cell r="T36"/>
+        </row>
         <row r="37">
           <cell r="A37" t="str">
             <v>MLA854432215</v>
@@ -2315,6 +2580,29 @@
           <cell r="S39">
             <v>141</v>
           </cell>
+          <cell r="T39"/>
+        </row>
+        <row r="40">
+          <cell r="A40"/>
+          <cell r="B40"/>
+          <cell r="C40"/>
+          <cell r="D40"/>
+          <cell r="E40"/>
+          <cell r="F40"/>
+          <cell r="G40"/>
+          <cell r="H40"/>
+          <cell r="I40"/>
+          <cell r="J40"/>
+          <cell r="K40"/>
+          <cell r="L40"/>
+          <cell r="M40"/>
+          <cell r="N40"/>
+          <cell r="O40"/>
+          <cell r="P40"/>
+          <cell r="Q40"/>
+          <cell r="R40"/>
+          <cell r="S40"/>
+          <cell r="T40"/>
         </row>
         <row r="41">
           <cell r="A41" t="str">
@@ -2441,9 +2729,182 @@
           </cell>
         </row>
         <row r="43">
+          <cell r="A43"/>
+          <cell r="B43"/>
+          <cell r="C43"/>
+          <cell r="D43"/>
+          <cell r="E43"/>
+          <cell r="F43"/>
+          <cell r="G43"/>
+          <cell r="H43"/>
+          <cell r="I43"/>
+          <cell r="J43"/>
+          <cell r="K43"/>
+          <cell r="L43"/>
+          <cell r="M43"/>
+          <cell r="N43"/>
+          <cell r="O43"/>
+          <cell r="P43"/>
+          <cell r="Q43"/>
+          <cell r="R43"/>
+          <cell r="S43"/>
           <cell r="T43">
             <v>6000010</v>
           </cell>
+        </row>
+        <row r="44">
+          <cell r="A44"/>
+          <cell r="B44"/>
+          <cell r="C44"/>
+          <cell r="D44"/>
+          <cell r="E44"/>
+          <cell r="F44"/>
+          <cell r="G44"/>
+          <cell r="H44"/>
+          <cell r="I44"/>
+          <cell r="J44"/>
+          <cell r="K44"/>
+          <cell r="L44"/>
+          <cell r="M44"/>
+          <cell r="N44"/>
+          <cell r="O44"/>
+          <cell r="P44"/>
+          <cell r="Q44"/>
+          <cell r="R44"/>
+          <cell r="S44"/>
+          <cell r="T44"/>
+        </row>
+        <row r="45">
+          <cell r="A45"/>
+          <cell r="B45"/>
+          <cell r="C45"/>
+          <cell r="D45"/>
+          <cell r="E45"/>
+          <cell r="F45"/>
+          <cell r="G45"/>
+          <cell r="H45"/>
+          <cell r="I45"/>
+          <cell r="J45"/>
+          <cell r="K45"/>
+          <cell r="L45"/>
+          <cell r="M45"/>
+          <cell r="N45"/>
+          <cell r="O45"/>
+          <cell r="P45"/>
+          <cell r="Q45"/>
+          <cell r="R45"/>
+          <cell r="S45"/>
+          <cell r="T45"/>
+        </row>
+        <row r="46">
+          <cell r="A46"/>
+          <cell r="B46"/>
+          <cell r="C46"/>
+          <cell r="D46"/>
+          <cell r="E46"/>
+          <cell r="F46"/>
+          <cell r="G46"/>
+          <cell r="H46"/>
+          <cell r="I46"/>
+          <cell r="J46"/>
+          <cell r="K46"/>
+          <cell r="L46"/>
+          <cell r="M46"/>
+          <cell r="N46"/>
+          <cell r="O46"/>
+          <cell r="P46"/>
+          <cell r="Q46"/>
+          <cell r="R46"/>
+          <cell r="S46"/>
+          <cell r="T46"/>
+        </row>
+        <row r="47">
+          <cell r="A47"/>
+          <cell r="B47"/>
+          <cell r="C47"/>
+          <cell r="D47"/>
+          <cell r="E47"/>
+          <cell r="F47"/>
+          <cell r="G47"/>
+          <cell r="H47"/>
+          <cell r="I47"/>
+          <cell r="J47"/>
+          <cell r="K47"/>
+          <cell r="L47"/>
+          <cell r="M47"/>
+          <cell r="N47"/>
+          <cell r="O47"/>
+          <cell r="P47"/>
+          <cell r="Q47"/>
+          <cell r="R47"/>
+          <cell r="S47"/>
+          <cell r="T47"/>
+        </row>
+        <row r="48">
+          <cell r="A48"/>
+          <cell r="B48"/>
+          <cell r="C48"/>
+          <cell r="D48"/>
+          <cell r="E48"/>
+          <cell r="F48"/>
+          <cell r="G48"/>
+          <cell r="H48"/>
+          <cell r="I48"/>
+          <cell r="J48"/>
+          <cell r="K48"/>
+          <cell r="L48"/>
+          <cell r="M48"/>
+          <cell r="N48"/>
+          <cell r="O48"/>
+          <cell r="P48"/>
+          <cell r="Q48"/>
+          <cell r="R48"/>
+          <cell r="S48"/>
+          <cell r="T48"/>
+        </row>
+        <row r="49">
+          <cell r="A49"/>
+          <cell r="B49"/>
+          <cell r="C49"/>
+          <cell r="D49"/>
+          <cell r="E49"/>
+          <cell r="F49"/>
+          <cell r="G49"/>
+          <cell r="H49"/>
+          <cell r="I49"/>
+          <cell r="J49"/>
+          <cell r="K49"/>
+          <cell r="L49"/>
+          <cell r="M49"/>
+          <cell r="N49"/>
+          <cell r="O49"/>
+          <cell r="P49"/>
+          <cell r="Q49"/>
+          <cell r="R49"/>
+          <cell r="S49"/>
+          <cell r="T49"/>
+        </row>
+        <row r="50">
+          <cell r="A50"/>
+          <cell r="B50"/>
+          <cell r="C50"/>
+          <cell r="D50"/>
+          <cell r="E50"/>
+          <cell r="F50"/>
+          <cell r="G50"/>
+          <cell r="H50"/>
+          <cell r="I50"/>
+          <cell r="J50"/>
+          <cell r="K50"/>
+          <cell r="L50"/>
+          <cell r="M50"/>
+          <cell r="N50"/>
+          <cell r="O50"/>
+          <cell r="P50"/>
+          <cell r="Q50"/>
+          <cell r="R50"/>
+          <cell r="S50"/>
+          <cell r="T50"/>
         </row>
         <row r="51">
           <cell r="A51" t="str">
@@ -2941,6 +3402,28 @@
             <v>Crear</v>
           </cell>
         </row>
+        <row r="59">
+          <cell r="A59"/>
+          <cell r="B59"/>
+          <cell r="C59"/>
+          <cell r="D59"/>
+          <cell r="E59"/>
+          <cell r="F59"/>
+          <cell r="G59"/>
+          <cell r="H59"/>
+          <cell r="I59"/>
+          <cell r="J59"/>
+          <cell r="K59"/>
+          <cell r="L59"/>
+          <cell r="M59"/>
+          <cell r="N59"/>
+          <cell r="O59"/>
+          <cell r="P59"/>
+          <cell r="Q59"/>
+          <cell r="R59"/>
+          <cell r="S59"/>
+          <cell r="T59"/>
+        </row>
         <row r="60">
           <cell r="A60" t="str">
             <v>MLA830418279</v>
@@ -3314,10 +3797,10 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4" refreshError="1"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>

</xml_diff>